<commit_message>
add arctic fox seqs
</commit_message>
<xml_diff>
--- a/output_data/Codon_usage_N.xlsx
+++ b/output_data/Codon_usage_N.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rowandurrant/Documents/GitHub/rabies-codon-bias/output_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23ADC8F-B77B-CC48-B532-5366FF8690F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8544A8C-A525-EE49-911F-3CE406BBDD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="2880" windowWidth="24240" windowHeight="13140" xr2:uid="{B2E6A4CB-E560-41F3-82E4-93FE4151198E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="509">
   <si>
     <t>CODONS</t>
   </si>
@@ -1549,6 +1549,21 @@
   <si>
     <t>MN384717</t>
   </si>
+  <si>
+    <t>AY352487</t>
+  </si>
+  <si>
+    <t>EF611828</t>
+  </si>
+  <si>
+    <t>EF611830</t>
+  </si>
+  <si>
+    <t>EF611851</t>
+  </si>
+  <si>
+    <t>L20675</t>
+  </si>
 </sst>
 </file>
 
@@ -1899,10 +1914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC27F32-A78F-4874-8508-5910ADF27ABB}">
-  <dimension ref="A1:BH427"/>
+  <dimension ref="A1:BH432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BJ1" sqref="BI1:BJ1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
+      <selection activeCell="F433" sqref="F433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -79625,6 +79640,916 @@
         <v>14</v>
       </c>
     </row>
+    <row r="428" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
+        <v>504</v>
+      </c>
+      <c r="B428">
+        <v>10</v>
+      </c>
+      <c r="C428">
+        <v>17</v>
+      </c>
+      <c r="D428">
+        <v>4</v>
+      </c>
+      <c r="E428">
+        <v>9</v>
+      </c>
+      <c r="F428">
+        <v>3</v>
+      </c>
+      <c r="G428">
+        <v>3</v>
+      </c>
+      <c r="H428">
+        <v>5</v>
+      </c>
+      <c r="I428">
+        <v>11</v>
+      </c>
+      <c r="J428">
+        <v>9</v>
+      </c>
+      <c r="K428">
+        <v>9</v>
+      </c>
+      <c r="L428">
+        <v>9</v>
+      </c>
+      <c r="M428">
+        <v>6</v>
+      </c>
+      <c r="N428">
+        <v>9</v>
+      </c>
+      <c r="O428">
+        <v>6</v>
+      </c>
+      <c r="P428">
+        <v>6</v>
+      </c>
+      <c r="Q428">
+        <v>7</v>
+      </c>
+      <c r="R428">
+        <v>5</v>
+      </c>
+      <c r="S428">
+        <v>10</v>
+      </c>
+      <c r="T428">
+        <v>4</v>
+      </c>
+      <c r="U428">
+        <v>4</v>
+      </c>
+      <c r="V428">
+        <v>5</v>
+      </c>
+      <c r="W428">
+        <v>7</v>
+      </c>
+      <c r="X428">
+        <v>5</v>
+      </c>
+      <c r="Y428">
+        <v>5</v>
+      </c>
+      <c r="Z428">
+        <v>0</v>
+      </c>
+      <c r="AA428">
+        <v>8</v>
+      </c>
+      <c r="AB428">
+        <v>8</v>
+      </c>
+      <c r="AC428">
+        <v>4</v>
+      </c>
+      <c r="AD428">
+        <v>9</v>
+      </c>
+      <c r="AE428">
+        <v>12</v>
+      </c>
+      <c r="AF428">
+        <v>6</v>
+      </c>
+      <c r="AG428">
+        <v>15</v>
+      </c>
+      <c r="AH428">
+        <v>1</v>
+      </c>
+      <c r="AI428">
+        <v>15</v>
+      </c>
+      <c r="AJ428">
+        <v>6</v>
+      </c>
+      <c r="AK428">
+        <v>6</v>
+      </c>
+      <c r="AL428">
+        <v>7</v>
+      </c>
+      <c r="AM428">
+        <v>6</v>
+      </c>
+      <c r="AN428">
+        <v>4</v>
+      </c>
+      <c r="AO428">
+        <v>10</v>
+      </c>
+      <c r="AP428">
+        <v>10</v>
+      </c>
+      <c r="AQ428">
+        <v>7</v>
+      </c>
+      <c r="AR428">
+        <v>19</v>
+      </c>
+      <c r="AS428">
+        <v>12</v>
+      </c>
+      <c r="AT428">
+        <v>11</v>
+      </c>
+      <c r="AU428">
+        <v>9</v>
+      </c>
+      <c r="AV428">
+        <v>23</v>
+      </c>
+      <c r="AW428">
+        <v>4</v>
+      </c>
+      <c r="AX428">
+        <v>2</v>
+      </c>
+      <c r="AY428">
+        <v>3</v>
+      </c>
+      <c r="AZ428">
+        <v>0</v>
+      </c>
+      <c r="BA428">
+        <v>1</v>
+      </c>
+      <c r="BB428">
+        <v>3</v>
+      </c>
+      <c r="BC428">
+        <v>12</v>
+      </c>
+      <c r="BD428">
+        <v>4</v>
+      </c>
+      <c r="BE428">
+        <v>5</v>
+      </c>
+      <c r="BF428">
+        <v>4</v>
+      </c>
+      <c r="BG428">
+        <v>8</v>
+      </c>
+      <c r="BH428">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="429" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A429" t="s">
+        <v>505</v>
+      </c>
+      <c r="B429">
+        <v>10</v>
+      </c>
+      <c r="C429">
+        <v>17</v>
+      </c>
+      <c r="D429">
+        <v>4</v>
+      </c>
+      <c r="E429">
+        <v>10</v>
+      </c>
+      <c r="F429">
+        <v>3</v>
+      </c>
+      <c r="G429">
+        <v>3</v>
+      </c>
+      <c r="H429">
+        <v>5</v>
+      </c>
+      <c r="I429">
+        <v>10</v>
+      </c>
+      <c r="J429">
+        <v>10</v>
+      </c>
+      <c r="K429">
+        <v>8</v>
+      </c>
+      <c r="L429">
+        <v>9</v>
+      </c>
+      <c r="M429">
+        <v>6</v>
+      </c>
+      <c r="N429">
+        <v>9</v>
+      </c>
+      <c r="O429">
+        <v>6</v>
+      </c>
+      <c r="P429">
+        <v>6</v>
+      </c>
+      <c r="Q429">
+        <v>6</v>
+      </c>
+      <c r="R429">
+        <v>5</v>
+      </c>
+      <c r="S429">
+        <v>10</v>
+      </c>
+      <c r="T429">
+        <v>5</v>
+      </c>
+      <c r="U429">
+        <v>5</v>
+      </c>
+      <c r="V429">
+        <v>4</v>
+      </c>
+      <c r="W429">
+        <v>7</v>
+      </c>
+      <c r="X429">
+        <v>5</v>
+      </c>
+      <c r="Y429">
+        <v>5</v>
+      </c>
+      <c r="Z429">
+        <v>0</v>
+      </c>
+      <c r="AA429">
+        <v>9</v>
+      </c>
+      <c r="AB429">
+        <v>7</v>
+      </c>
+      <c r="AC429">
+        <v>5</v>
+      </c>
+      <c r="AD429">
+        <v>9</v>
+      </c>
+      <c r="AE429">
+        <v>11</v>
+      </c>
+      <c r="AF429">
+        <v>7</v>
+      </c>
+      <c r="AG429">
+        <v>14</v>
+      </c>
+      <c r="AH429">
+        <v>1</v>
+      </c>
+      <c r="AI429">
+        <v>15</v>
+      </c>
+      <c r="AJ429">
+        <v>6</v>
+      </c>
+      <c r="AK429">
+        <v>6</v>
+      </c>
+      <c r="AL429">
+        <v>7</v>
+      </c>
+      <c r="AM429">
+        <v>6</v>
+      </c>
+      <c r="AN429">
+        <v>4</v>
+      </c>
+      <c r="AO429">
+        <v>9</v>
+      </c>
+      <c r="AP429">
+        <v>11</v>
+      </c>
+      <c r="AQ429">
+        <v>7</v>
+      </c>
+      <c r="AR429">
+        <v>19</v>
+      </c>
+      <c r="AS429">
+        <v>12</v>
+      </c>
+      <c r="AT429">
+        <v>11</v>
+      </c>
+      <c r="AU429">
+        <v>9</v>
+      </c>
+      <c r="AV429">
+        <v>23</v>
+      </c>
+      <c r="AW429">
+        <v>4</v>
+      </c>
+      <c r="AX429">
+        <v>2</v>
+      </c>
+      <c r="AY429">
+        <v>3</v>
+      </c>
+      <c r="AZ429">
+        <v>0</v>
+      </c>
+      <c r="BA429">
+        <v>1</v>
+      </c>
+      <c r="BB429">
+        <v>3</v>
+      </c>
+      <c r="BC429">
+        <v>12</v>
+      </c>
+      <c r="BD429">
+        <v>4</v>
+      </c>
+      <c r="BE429">
+        <v>5</v>
+      </c>
+      <c r="BF429">
+        <v>4</v>
+      </c>
+      <c r="BG429">
+        <v>8</v>
+      </c>
+      <c r="BH429">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="430" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A430" t="s">
+        <v>506</v>
+      </c>
+      <c r="B430">
+        <v>10</v>
+      </c>
+      <c r="C430">
+        <v>17</v>
+      </c>
+      <c r="D430">
+        <v>4</v>
+      </c>
+      <c r="E430">
+        <v>9</v>
+      </c>
+      <c r="F430">
+        <v>3</v>
+      </c>
+      <c r="G430">
+        <v>3</v>
+      </c>
+      <c r="H430">
+        <v>5</v>
+      </c>
+      <c r="I430">
+        <v>11</v>
+      </c>
+      <c r="J430">
+        <v>9</v>
+      </c>
+      <c r="K430">
+        <v>9</v>
+      </c>
+      <c r="L430">
+        <v>9</v>
+      </c>
+      <c r="M430">
+        <v>6</v>
+      </c>
+      <c r="N430">
+        <v>9</v>
+      </c>
+      <c r="O430">
+        <v>6</v>
+      </c>
+      <c r="P430">
+        <v>6</v>
+      </c>
+      <c r="Q430">
+        <v>7</v>
+      </c>
+      <c r="R430">
+        <v>5</v>
+      </c>
+      <c r="S430">
+        <v>10</v>
+      </c>
+      <c r="T430">
+        <v>4</v>
+      </c>
+      <c r="U430">
+        <v>4</v>
+      </c>
+      <c r="V430">
+        <v>5</v>
+      </c>
+      <c r="W430">
+        <v>7</v>
+      </c>
+      <c r="X430">
+        <v>5</v>
+      </c>
+      <c r="Y430">
+        <v>5</v>
+      </c>
+      <c r="Z430">
+        <v>0</v>
+      </c>
+      <c r="AA430">
+        <v>8</v>
+      </c>
+      <c r="AB430">
+        <v>8</v>
+      </c>
+      <c r="AC430">
+        <v>5</v>
+      </c>
+      <c r="AD430">
+        <v>9</v>
+      </c>
+      <c r="AE430">
+        <v>12</v>
+      </c>
+      <c r="AF430">
+        <v>6</v>
+      </c>
+      <c r="AG430">
+        <v>14</v>
+      </c>
+      <c r="AH430">
+        <v>1</v>
+      </c>
+      <c r="AI430">
+        <v>15</v>
+      </c>
+      <c r="AJ430">
+        <v>6</v>
+      </c>
+      <c r="AK430">
+        <v>6</v>
+      </c>
+      <c r="AL430">
+        <v>7</v>
+      </c>
+      <c r="AM430">
+        <v>6</v>
+      </c>
+      <c r="AN430">
+        <v>4</v>
+      </c>
+      <c r="AO430">
+        <v>10</v>
+      </c>
+      <c r="AP430">
+        <v>10</v>
+      </c>
+      <c r="AQ430">
+        <v>6</v>
+      </c>
+      <c r="AR430">
+        <v>20</v>
+      </c>
+      <c r="AS430">
+        <v>12</v>
+      </c>
+      <c r="AT430">
+        <v>11</v>
+      </c>
+      <c r="AU430">
+        <v>9</v>
+      </c>
+      <c r="AV430">
+        <v>23</v>
+      </c>
+      <c r="AW430">
+        <v>4</v>
+      </c>
+      <c r="AX430">
+        <v>2</v>
+      </c>
+      <c r="AY430">
+        <v>3</v>
+      </c>
+      <c r="AZ430">
+        <v>0</v>
+      </c>
+      <c r="BA430">
+        <v>1</v>
+      </c>
+      <c r="BB430">
+        <v>3</v>
+      </c>
+      <c r="BC430">
+        <v>12</v>
+      </c>
+      <c r="BD430">
+        <v>4</v>
+      </c>
+      <c r="BE430">
+        <v>5</v>
+      </c>
+      <c r="BF430">
+        <v>4</v>
+      </c>
+      <c r="BG430">
+        <v>7</v>
+      </c>
+      <c r="BH430">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="431" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
+        <v>507</v>
+      </c>
+      <c r="B431">
+        <v>10</v>
+      </c>
+      <c r="C431">
+        <v>17</v>
+      </c>
+      <c r="D431">
+        <v>2</v>
+      </c>
+      <c r="E431">
+        <v>10</v>
+      </c>
+      <c r="F431">
+        <v>4</v>
+      </c>
+      <c r="G431">
+        <v>3</v>
+      </c>
+      <c r="H431">
+        <v>6</v>
+      </c>
+      <c r="I431">
+        <v>10</v>
+      </c>
+      <c r="J431">
+        <v>10</v>
+      </c>
+      <c r="K431">
+        <v>8</v>
+      </c>
+      <c r="L431">
+        <v>9</v>
+      </c>
+      <c r="M431">
+        <v>8</v>
+      </c>
+      <c r="N431">
+        <v>7</v>
+      </c>
+      <c r="O431">
+        <v>6</v>
+      </c>
+      <c r="P431">
+        <v>6</v>
+      </c>
+      <c r="Q431">
+        <v>8</v>
+      </c>
+      <c r="R431">
+        <v>4</v>
+      </c>
+      <c r="S431">
+        <v>10</v>
+      </c>
+      <c r="T431">
+        <v>4</v>
+      </c>
+      <c r="U431">
+        <v>5</v>
+      </c>
+      <c r="V431">
+        <v>4</v>
+      </c>
+      <c r="W431">
+        <v>7</v>
+      </c>
+      <c r="X431">
+        <v>5</v>
+      </c>
+      <c r="Y431">
+        <v>5</v>
+      </c>
+      <c r="Z431">
+        <v>0</v>
+      </c>
+      <c r="AA431">
+        <v>12</v>
+      </c>
+      <c r="AB431">
+        <v>5</v>
+      </c>
+      <c r="AC431">
+        <v>5</v>
+      </c>
+      <c r="AD431">
+        <v>8</v>
+      </c>
+      <c r="AE431">
+        <v>11</v>
+      </c>
+      <c r="AF431">
+        <v>7</v>
+      </c>
+      <c r="AG431">
+        <v>14</v>
+      </c>
+      <c r="AH431">
+        <v>1</v>
+      </c>
+      <c r="AI431">
+        <v>16</v>
+      </c>
+      <c r="AJ431">
+        <v>5</v>
+      </c>
+      <c r="AK431">
+        <v>6</v>
+      </c>
+      <c r="AL431">
+        <v>7</v>
+      </c>
+      <c r="AM431">
+        <v>6</v>
+      </c>
+      <c r="AN431">
+        <v>4</v>
+      </c>
+      <c r="AO431">
+        <v>12</v>
+      </c>
+      <c r="AP431">
+        <v>8</v>
+      </c>
+      <c r="AQ431">
+        <v>5</v>
+      </c>
+      <c r="AR431">
+        <v>21</v>
+      </c>
+      <c r="AS431">
+        <v>12</v>
+      </c>
+      <c r="AT431">
+        <v>11</v>
+      </c>
+      <c r="AU431">
+        <v>11</v>
+      </c>
+      <c r="AV431">
+        <v>21</v>
+      </c>
+      <c r="AW431">
+        <v>4</v>
+      </c>
+      <c r="AX431">
+        <v>2</v>
+      </c>
+      <c r="AY431">
+        <v>3</v>
+      </c>
+      <c r="AZ431">
+        <v>0</v>
+      </c>
+      <c r="BA431">
+        <v>1</v>
+      </c>
+      <c r="BB431">
+        <v>3</v>
+      </c>
+      <c r="BC431">
+        <v>13</v>
+      </c>
+      <c r="BD431">
+        <v>3</v>
+      </c>
+      <c r="BE431">
+        <v>7</v>
+      </c>
+      <c r="BF431">
+        <v>3</v>
+      </c>
+      <c r="BG431">
+        <v>9</v>
+      </c>
+      <c r="BH431">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="432" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A432" t="s">
+        <v>508</v>
+      </c>
+      <c r="B432">
+        <v>10</v>
+      </c>
+      <c r="C432">
+        <v>17</v>
+      </c>
+      <c r="D432">
+        <v>4</v>
+      </c>
+      <c r="E432">
+        <v>9</v>
+      </c>
+      <c r="F432">
+        <v>3</v>
+      </c>
+      <c r="G432">
+        <v>3</v>
+      </c>
+      <c r="H432">
+        <v>4</v>
+      </c>
+      <c r="I432">
+        <v>12</v>
+      </c>
+      <c r="J432">
+        <v>11</v>
+      </c>
+      <c r="K432">
+        <v>7</v>
+      </c>
+      <c r="L432">
+        <v>9</v>
+      </c>
+      <c r="M432">
+        <v>7</v>
+      </c>
+      <c r="N432">
+        <v>8</v>
+      </c>
+      <c r="O432">
+        <v>6</v>
+      </c>
+      <c r="P432">
+        <v>6</v>
+      </c>
+      <c r="Q432">
+        <v>7</v>
+      </c>
+      <c r="R432">
+        <v>6</v>
+      </c>
+      <c r="S432">
+        <v>9</v>
+      </c>
+      <c r="T432">
+        <v>3</v>
+      </c>
+      <c r="U432">
+        <v>4</v>
+      </c>
+      <c r="V432">
+        <v>5</v>
+      </c>
+      <c r="W432">
+        <v>7</v>
+      </c>
+      <c r="X432">
+        <v>5</v>
+      </c>
+      <c r="Y432">
+        <v>5</v>
+      </c>
+      <c r="Z432">
+        <v>1</v>
+      </c>
+      <c r="AA432">
+        <v>10</v>
+      </c>
+      <c r="AB432">
+        <v>6</v>
+      </c>
+      <c r="AC432">
+        <v>6</v>
+      </c>
+      <c r="AD432">
+        <v>7</v>
+      </c>
+      <c r="AE432">
+        <v>11</v>
+      </c>
+      <c r="AF432">
+        <v>7</v>
+      </c>
+      <c r="AG432">
+        <v>14</v>
+      </c>
+      <c r="AH432">
+        <v>2</v>
+      </c>
+      <c r="AI432">
+        <v>14</v>
+      </c>
+      <c r="AJ432">
+        <v>7</v>
+      </c>
+      <c r="AK432">
+        <v>6</v>
+      </c>
+      <c r="AL432">
+        <v>7</v>
+      </c>
+      <c r="AM432">
+        <v>6</v>
+      </c>
+      <c r="AN432">
+        <v>4</v>
+      </c>
+      <c r="AO432">
+        <v>9</v>
+      </c>
+      <c r="AP432">
+        <v>12</v>
+      </c>
+      <c r="AQ432">
+        <v>7</v>
+      </c>
+      <c r="AR432">
+        <v>18</v>
+      </c>
+      <c r="AS432">
+        <v>12</v>
+      </c>
+      <c r="AT432">
+        <v>11</v>
+      </c>
+      <c r="AU432">
+        <v>11</v>
+      </c>
+      <c r="AV432">
+        <v>21</v>
+      </c>
+      <c r="AW432">
+        <v>4</v>
+      </c>
+      <c r="AX432">
+        <v>2</v>
+      </c>
+      <c r="AY432">
+        <v>3</v>
+      </c>
+      <c r="AZ432">
+        <v>0</v>
+      </c>
+      <c r="BA432">
+        <v>1</v>
+      </c>
+      <c r="BB432">
+        <v>3</v>
+      </c>
+      <c r="BC432">
+        <v>12</v>
+      </c>
+      <c r="BD432">
+        <v>4</v>
+      </c>
+      <c r="BE432">
+        <v>5</v>
+      </c>
+      <c r="BF432">
+        <v>3</v>
+      </c>
+      <c r="BG432">
+        <v>10</v>
+      </c>
+      <c r="BH432">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>